<commit_message>
Fixed error with Inland Empire place ID and reanalyzed data assuming IE is the average of San Bernardino and Riverside counties
</commit_message>
<xml_diff>
--- a/figures/table 1.xlsx
+++ b/figures/table 1.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Google Drive\Research\CNC Lichens\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050EAEC5-D269-422F-88E0-692B6748D7FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F58AD5-1D2B-470C-949F-B195B8054E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="380" windowWidth="17590" windowHeight="8570" activeTab="1" xr2:uid="{88CF4EEC-E34F-49DB-A7BB-E30DB657DA0B}"/>
+    <workbookView xWindow="4380" yWindow="-15480" windowWidth="19455" windowHeight="14460" activeTab="1" xr2:uid="{88CF4EEC-E34F-49DB-A7BB-E30DB657DA0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="csv version" sheetId="2" r:id="rId2"/>
+    <sheet name="table 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Observations</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Inland Empire</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -196,16 +199,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -526,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5908866E-0B6D-4C48-B3C5-EDDC3FFBA3C2}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -559,7 +576,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2">
@@ -597,7 +614,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3">
         <v>2020</v>
       </c>
@@ -608,18 +625,18 @@
         <v>31450</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E11" si="0">C3/D3</f>
+        <f t="shared" ref="E3:E12" si="0">C3/D3</f>
         <v>1.4085850556438791E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H3" s="1">
         <v>2496</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ref="I3:I11" si="1">G3/H3</f>
-        <v>5.128205128205128E-2</v>
+        <v>5.1682692307692304E-2</v>
       </c>
       <c r="K3" s="1">
         <v>112</v>
@@ -633,7 +650,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -671,7 +688,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5">
         <v>2020</v>
       </c>
@@ -707,7 +724,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -745,7 +762,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7">
         <v>2020</v>
       </c>
@@ -781,7 +798,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -819,7 +836,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9">
         <v>2020</v>
       </c>
@@ -928,6 +945,46 @@
       <c r="M11" s="2">
         <f t="shared" si="2"/>
         <v>1.9230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12" s="3">
+        <v>81</v>
+      </c>
+      <c r="D12" s="3">
+        <v>10899</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4318744838976049E-3</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3">
+        <v>18</v>
+      </c>
+      <c r="H12" s="3">
+        <v>485</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" ref="I12" si="3">G12/H12</f>
+        <v>3.711340206185567E-2</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="3">
+        <v>38</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1835</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" ref="M12" si="4">K12/L12</f>
+        <v>2.0708446866485014E-2</v>
       </c>
     </row>
   </sheetData>
@@ -943,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B013A97C-3F41-4568-8226-8EC690CA7C9D}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1038,18 +1095,18 @@
         <v>31450</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E11" si="0">C3/D3</f>
+        <f t="shared" ref="E3:E12" si="0">C3/D3</f>
         <v>1.4085850556438791E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G3" s="1">
         <v>2496</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H11" si="1">F3/G3</f>
-        <v>5.128205128205128E-2</v>
+        <f t="shared" ref="H3:H12" si="1">F3/G3</f>
+        <v>5.1682692307692304E-2</v>
       </c>
       <c r="I3" s="1">
         <v>112</v>
@@ -1058,7 +1115,7 @@
         <v>2975</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K11" si="2">I3/J3</f>
+        <f t="shared" ref="K3:K12" si="2">I3/J3</f>
         <v>3.7647058823529408E-2</v>
       </c>
     </row>
@@ -1364,6 +1421,44 @@
       <c r="K11" s="2">
         <f t="shared" si="2"/>
         <v>1.9230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12" s="3">
+        <v>81</v>
+      </c>
+      <c r="D12" s="3">
+        <v>10899</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4318744838976049E-3</v>
+      </c>
+      <c r="F12" s="3">
+        <v>18</v>
+      </c>
+      <c r="G12" s="3">
+        <v>485</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>3.711340206185567E-2</v>
+      </c>
+      <c r="I12" s="3">
+        <v>38</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1835</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="2"/>
+        <v>2.0708446866485014E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>